<commit_message>
added exp 1.2 finished
</commit_message>
<xml_diff>
--- a/data/exp1.2/2023_Aug18_salbutamolexp1_2_meta.xlsx
+++ b/data/exp1.2/2023_Aug18_salbutamolexp1_2_meta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karissabarthelson/Documents/2023_MPSIII_salbutamol/data/exp1.2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7EFCAF-55D5-A743-BB97-FBB3800CA11F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983D05AB-4166-4B4B-A3E3-7A1E07F452DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32420" yWindow="-5140" windowWidth="25000" windowHeight="19320" xr2:uid="{BD720F60-64AD-4D4B-861E-3C9FD6A3C16A}"/>
+    <workbookView xWindow="38560" yWindow="-11760" windowWidth="25000" windowHeight="19320" xr2:uid="{BD720F60-64AD-4D4B-861E-3C9FD6A3C16A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="161">
   <si>
     <t>fish_id</t>
   </si>
@@ -412,13 +412,121 @@
   </si>
   <si>
     <t>tube</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230818T104225.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230818T115512.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230818T130756.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230818T141841.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230818T153026.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230818T164047.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230818T104448.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230818T115819.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230818T131031.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230818T142116.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230818T153317.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230818T164456.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230818T104226-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230818T115513-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230818T130757-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230818T141842-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230818T153027-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230818T164048-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230818T104449-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230818T115820-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230818T131032-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230818T142117-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230818T153318-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230818T164456-data_totals.csv</t>
+  </si>
+  <si>
+    <t>YMaze_tracking139-20230818T104257-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking139-20230818T115543-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking139-20230818T130827-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking139-20230818T141912-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking139-20230818T153057-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking139-20230818T164118-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking-20230818T104519-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking-20230818T115850-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking-20230818T131102-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking-20230818T142147-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking-20230818T153348-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking-20230818T164526-f30.avi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -447,6 +555,31 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFF8F8F2"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -653,7 +786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -719,6 +852,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1741,9 +1878,9 @@
   </sheetPr>
   <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M96" sqref="M96"/>
+      <selection pane="topRight" activeCell="J91" sqref="J91:J95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1823,9 +1960,15 @@
       <c r="G2" s="17">
         <v>1</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="H2" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="K2" s="9"/>
       <c r="L2" s="10"/>
       <c r="M2" s="9" t="s">
@@ -1854,9 +1997,15 @@
       <c r="G3" s="19">
         <v>2</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="H3" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="K3" s="9"/>
       <c r="L3" s="10"/>
       <c r="M3" s="9" t="s">
@@ -1885,9 +2034,15 @@
       <c r="G4" s="19">
         <v>3</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="H4" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="K4" s="9"/>
       <c r="L4" s="10"/>
       <c r="M4" s="9" t="s">
@@ -1916,9 +2071,15 @@
       <c r="G5" s="19">
         <v>4</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="H5" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="K5" s="9"/>
       <c r="L5" s="10"/>
       <c r="M5" s="9" t="s">
@@ -1947,9 +2108,15 @@
       <c r="G6" s="19">
         <v>5</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="H6" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="K6" s="9"/>
       <c r="L6" s="10"/>
       <c r="M6" s="9" t="s">
@@ -1978,9 +2145,15 @@
       <c r="G7" s="19">
         <v>6</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="H7" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="K7" s="9"/>
       <c r="L7" s="10"/>
       <c r="M7" s="9" t="s">
@@ -2009,9 +2182,15 @@
       <c r="G8" s="19">
         <v>7</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="H8" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="K8" s="9"/>
       <c r="L8" s="10"/>
       <c r="M8" s="9" t="s">
@@ -2040,9 +2219,15 @@
       <c r="G9" s="23">
         <v>8</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="H9" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="K9" s="9"/>
       <c r="L9" s="10"/>
       <c r="M9" s="9" t="s">
@@ -2071,9 +2256,15 @@
       <c r="G10" s="17">
         <v>1</v>
       </c>
-      <c r="H10" s="24"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="H10" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>155</v>
+      </c>
       <c r="K10" s="9"/>
       <c r="L10" s="10"/>
       <c r="M10" s="9" t="s">
@@ -2102,9 +2293,15 @@
       <c r="G11" s="19">
         <v>2</v>
       </c>
-      <c r="H11" s="24"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="H11" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>155</v>
+      </c>
       <c r="K11" s="9"/>
       <c r="L11" s="10"/>
       <c r="M11" s="9" t="s">
@@ -2133,9 +2330,15 @@
       <c r="G12" s="19">
         <v>3</v>
       </c>
-      <c r="H12" s="24"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="H12" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>155</v>
+      </c>
       <c r="K12" s="9"/>
       <c r="L12" s="10"/>
       <c r="M12" s="9" t="s">
@@ -2164,9 +2367,15 @@
       <c r="G13" s="19">
         <v>4</v>
       </c>
-      <c r="H13" s="24"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="H13" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>155</v>
+      </c>
       <c r="K13" s="9"/>
       <c r="L13" s="10"/>
       <c r="M13" s="9" t="s">
@@ -2195,9 +2404,15 @@
       <c r="G14" s="19">
         <v>5</v>
       </c>
-      <c r="H14" s="24"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="H14" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>155</v>
+      </c>
       <c r="K14" s="9"/>
       <c r="L14" s="10"/>
       <c r="M14" s="9" t="s">
@@ -2226,9 +2441,15 @@
       <c r="G15" s="19">
         <v>6</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="H15" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>155</v>
+      </c>
       <c r="K15" s="9"/>
       <c r="L15" s="10"/>
       <c r="M15" s="9" t="s">
@@ -2257,9 +2478,15 @@
       <c r="G16" s="19">
         <v>7</v>
       </c>
-      <c r="H16" s="24"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
+      <c r="H16" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>155</v>
+      </c>
       <c r="K16" s="9"/>
       <c r="L16" s="10"/>
       <c r="M16" s="9" t="s">
@@ -2288,9 +2515,15 @@
       <c r="G17" s="23">
         <v>8</v>
       </c>
-      <c r="H17" s="24"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
+      <c r="H17" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>155</v>
+      </c>
       <c r="K17" s="9"/>
       <c r="L17" s="10"/>
       <c r="M17" s="9" t="s">
@@ -2319,9 +2552,15 @@
       <c r="G18" s="17">
         <v>1</v>
       </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
+      <c r="H18" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I18" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K18" s="9"/>
       <c r="L18" s="10"/>
       <c r="M18" s="9" t="s">
@@ -2350,9 +2589,15 @@
       <c r="G19" s="19">
         <v>2</v>
       </c>
-      <c r="H19" s="12"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
+      <c r="H19" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K19" s="9"/>
       <c r="L19" s="10"/>
       <c r="M19" s="9" t="s">
@@ -2381,9 +2626,15 @@
       <c r="G20" s="19">
         <v>3</v>
       </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
+      <c r="H20" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K20" s="9"/>
       <c r="L20" s="10"/>
       <c r="M20" s="9" t="s">
@@ -2412,9 +2663,15 @@
       <c r="G21" s="19">
         <v>4</v>
       </c>
-      <c r="H21" s="12"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
+      <c r="H21" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K21" s="9"/>
       <c r="L21" s="10"/>
       <c r="M21" s="9" t="s">
@@ -2443,9 +2700,15 @@
       <c r="G22" s="19">
         <v>5</v>
       </c>
-      <c r="H22" s="12"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
+      <c r="H22" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I22" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K22" s="9"/>
       <c r="L22" s="10"/>
       <c r="M22" s="9" t="s">
@@ -2474,9 +2737,15 @@
       <c r="G23" s="19">
         <v>6</v>
       </c>
-      <c r="H23" s="12"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
+      <c r="H23" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I23" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K23" s="9"/>
       <c r="L23" s="10"/>
       <c r="M23" s="9" t="s">
@@ -2505,9 +2774,15 @@
       <c r="G24" s="19">
         <v>7</v>
       </c>
-      <c r="H24" s="12"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
+      <c r="H24" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I24" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K24" s="9"/>
       <c r="L24" s="10"/>
       <c r="M24" s="9" t="s">
@@ -2536,9 +2811,15 @@
       <c r="G25" s="23">
         <v>8</v>
       </c>
-      <c r="H25" s="12"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="H25" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="K25" s="9"/>
       <c r="L25" s="10"/>
       <c r="M25" s="9" t="s">
@@ -2567,9 +2848,15 @@
       <c r="G26" s="13">
         <v>1</v>
       </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
+      <c r="H26" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>156</v>
+      </c>
       <c r="K26" s="9"/>
       <c r="L26" s="10"/>
       <c r="M26" s="9" t="s">
@@ -2598,9 +2885,15 @@
       <c r="G27" s="1">
         <v>2</v>
       </c>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
+      <c r="H27" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>156</v>
+      </c>
       <c r="K27" s="9"/>
       <c r="L27" s="10"/>
       <c r="M27" s="9" t="s">
@@ -2629,9 +2922,15 @@
       <c r="G28" s="1">
         <v>3</v>
       </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="H28" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>156</v>
+      </c>
       <c r="K28" s="9"/>
       <c r="L28" s="10"/>
       <c r="M28" s="9" t="s">
@@ -2660,9 +2959,15 @@
       <c r="G29" s="1">
         <v>4</v>
       </c>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
+      <c r="H29" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I29" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>156</v>
+      </c>
       <c r="K29" s="9"/>
       <c r="L29" s="10"/>
       <c r="M29" s="9" t="s">
@@ -2691,9 +2996,15 @@
       <c r="G30" s="1">
         <v>5</v>
       </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
+      <c r="H30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>156</v>
+      </c>
       <c r="K30" s="9"/>
       <c r="L30" s="10"/>
       <c r="M30" s="9" t="s">
@@ -2722,9 +3033,15 @@
       <c r="G31" s="1">
         <v>6</v>
       </c>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="H31" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I31" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>156</v>
+      </c>
       <c r="K31" s="9"/>
       <c r="L31" s="10"/>
       <c r="M31" s="9" t="s">
@@ -2753,9 +3070,15 @@
       <c r="G32" s="1">
         <v>7</v>
       </c>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
+      <c r="H32" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I32" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>156</v>
+      </c>
       <c r="K32" s="9"/>
       <c r="L32" s="10"/>
       <c r="M32" s="9" t="s">
@@ -2784,9 +3107,15 @@
       <c r="G33" s="1">
         <v>8</v>
       </c>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
+      <c r="H33" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I33" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>156</v>
+      </c>
       <c r="K33" s="9"/>
       <c r="L33" s="10"/>
       <c r="M33" s="9" t="s">
@@ -2815,9 +3144,15 @@
       <c r="G34" s="1">
         <v>1</v>
       </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
+      <c r="H34" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="I34" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="K34" s="9"/>
       <c r="L34" s="10"/>
       <c r="M34" s="9" t="s">
@@ -2846,9 +3181,15 @@
       <c r="G35" s="1">
         <v>2</v>
       </c>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
+      <c r="H35" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="I35" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="K35" s="9"/>
       <c r="L35" s="10"/>
       <c r="M35" s="9" t="s">
@@ -2877,9 +3218,15 @@
       <c r="G36" s="1">
         <v>3</v>
       </c>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
+      <c r="H36" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="I36" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="K36" s="9"/>
       <c r="L36" s="10"/>
       <c r="M36" s="9" t="s">
@@ -2908,9 +3255,15 @@
       <c r="G37" s="1">
         <v>4</v>
       </c>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
+      <c r="H37" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="I37" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="K37" s="9"/>
       <c r="L37" s="10"/>
       <c r="M37" s="9" t="s">
@@ -2939,9 +3292,15 @@
       <c r="G38" s="1">
         <v>5</v>
       </c>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
+      <c r="H38" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="I38" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="K38" s="9"/>
       <c r="L38" s="10"/>
       <c r="M38" s="9" t="s">
@@ -2970,9 +3329,15 @@
       <c r="G39" s="1">
         <v>6</v>
       </c>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
+      <c r="H39" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="I39" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="K39" s="9"/>
       <c r="L39" s="10"/>
       <c r="M39" s="9" t="s">
@@ -3001,9 +3366,15 @@
       <c r="G40" s="1">
         <v>7</v>
       </c>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
+      <c r="H40" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="I40" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="K40" s="9"/>
       <c r="L40" s="10"/>
       <c r="M40" s="9" t="s">
@@ -3032,9 +3403,15 @@
       <c r="G41" s="1">
         <v>8</v>
       </c>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
+      <c r="H41" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="K41" s="9"/>
       <c r="L41" s="10"/>
       <c r="M41" s="9" t="s">
@@ -3063,9 +3440,15 @@
       <c r="G42" s="1">
         <v>1</v>
       </c>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
+      <c r="H42" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I42" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>157</v>
+      </c>
       <c r="K42" s="9"/>
       <c r="L42" s="10"/>
       <c r="M42" s="9" t="s">
@@ -3094,9 +3477,15 @@
       <c r="G43" s="1">
         <v>2</v>
       </c>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
+      <c r="H43" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I43" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>157</v>
+      </c>
       <c r="K43" s="9"/>
       <c r="L43" s="10"/>
       <c r="M43" s="9" t="s">
@@ -3125,9 +3514,15 @@
       <c r="G44" s="1">
         <v>3</v>
       </c>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
+      <c r="H44" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I44" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>157</v>
+      </c>
       <c r="K44" s="9"/>
       <c r="L44" s="10"/>
       <c r="M44" s="9" t="s">
@@ -3156,9 +3551,15 @@
       <c r="G45" s="1">
         <v>4</v>
       </c>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
+      <c r="H45" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I45" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>157</v>
+      </c>
       <c r="K45" s="9"/>
       <c r="L45" s="10"/>
       <c r="M45" s="9" t="s">
@@ -3187,9 +3588,15 @@
       <c r="G46" s="1">
         <v>5</v>
       </c>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
+      <c r="H46" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I46" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>157</v>
+      </c>
       <c r="K46" s="9"/>
       <c r="L46" s="10"/>
       <c r="M46" s="9" t="s">
@@ -3218,9 +3625,15 @@
       <c r="G47" s="1">
         <v>6</v>
       </c>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
+      <c r="H47" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I47" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>157</v>
+      </c>
       <c r="K47" s="9"/>
       <c r="L47" s="10"/>
       <c r="M47" s="9" t="s">
@@ -3249,9 +3662,15 @@
       <c r="G48" s="1">
         <v>7</v>
       </c>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
+      <c r="H48" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I48" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="J48" s="8" t="s">
+        <v>157</v>
+      </c>
       <c r="K48" s="9"/>
       <c r="L48" s="10"/>
       <c r="M48" s="9" t="s">
@@ -3280,9 +3699,15 @@
       <c r="G49" s="1">
         <v>8</v>
       </c>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
+      <c r="H49" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I49" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="J49" s="8" t="s">
+        <v>157</v>
+      </c>
       <c r="K49" s="9"/>
       <c r="L49" s="10"/>
       <c r="M49" s="9" t="s">
@@ -3311,9 +3736,15 @@
       <c r="G50" s="1">
         <v>1</v>
       </c>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
+      <c r="H50" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I50" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="J50" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="K50" s="9"/>
       <c r="L50" s="10"/>
       <c r="M50" s="9" t="s">
@@ -3342,9 +3773,15 @@
       <c r="G51" s="1">
         <v>2</v>
       </c>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
+      <c r="H51" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I51" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="K51" s="9"/>
       <c r="L51" s="10"/>
       <c r="M51" s="9" t="s">
@@ -3373,9 +3810,15 @@
       <c r="G52" s="1">
         <v>3</v>
       </c>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
+      <c r="H52" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I52" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="K52" s="9"/>
       <c r="L52" s="10"/>
       <c r="M52" s="9" t="s">
@@ -3404,9 +3847,15 @@
       <c r="G53" s="1">
         <v>4</v>
       </c>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
+      <c r="H53" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I53" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="K53" s="9"/>
       <c r="L53" s="10"/>
       <c r="M53" s="9" t="s">
@@ -3435,9 +3884,15 @@
       <c r="G54" s="1">
         <v>5</v>
       </c>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
+      <c r="H54" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I54" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="K54" s="9"/>
       <c r="L54" s="10"/>
       <c r="M54" s="9" t="s">
@@ -3466,9 +3921,15 @@
       <c r="G55" s="1">
         <v>6</v>
       </c>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8"/>
+      <c r="H55" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I55" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="K55" s="9"/>
       <c r="L55" s="10"/>
       <c r="M55" s="9" t="s">
@@ -3497,9 +3958,15 @@
       <c r="G56" s="1">
         <v>7</v>
       </c>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
+      <c r="H56" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I56" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="J56" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="K56" s="9"/>
       <c r="L56" s="10"/>
       <c r="M56" s="9" t="s">
@@ -3528,9 +3995,15 @@
       <c r="G57" s="1">
         <v>8</v>
       </c>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
+      <c r="H57" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I57" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="J57" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="K57" s="9"/>
       <c r="L57" s="10"/>
       <c r="M57" s="9" t="s">
@@ -3559,9 +4032,15 @@
       <c r="G58" s="1">
         <v>1</v>
       </c>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
+      <c r="H58" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I58" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="J58" s="8" t="s">
+        <v>158</v>
+      </c>
       <c r="K58" s="9"/>
       <c r="L58" s="10"/>
       <c r="M58" s="9" t="s">
@@ -3590,9 +4069,15 @@
       <c r="G59" s="1">
         <v>2</v>
       </c>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8"/>
+      <c r="H59" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I59" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="J59" s="8" t="s">
+        <v>158</v>
+      </c>
       <c r="K59" s="9"/>
       <c r="L59" s="10"/>
       <c r="M59" s="9" t="s">
@@ -3621,9 +4106,15 @@
       <c r="G60" s="1">
         <v>3</v>
       </c>
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
+      <c r="H60" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I60" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="J60" s="8" t="s">
+        <v>158</v>
+      </c>
       <c r="K60" s="9"/>
       <c r="L60" s="10"/>
       <c r="M60" s="9" t="s">
@@ -3652,9 +4143,15 @@
       <c r="G61" s="1">
         <v>4</v>
       </c>
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
-      <c r="J61" s="8"/>
+      <c r="H61" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I61" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="J61" s="8" t="s">
+        <v>158</v>
+      </c>
       <c r="K61" s="9"/>
       <c r="L61" s="10"/>
       <c r="M61" s="9" t="s">
@@ -3683,9 +4180,15 @@
       <c r="G62" s="1">
         <v>5</v>
       </c>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
-      <c r="J62" s="8"/>
+      <c r="H62" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I62" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="J62" s="8" t="s">
+        <v>158</v>
+      </c>
       <c r="K62" s="9"/>
       <c r="L62" s="10"/>
       <c r="M62" s="9" t="s">
@@ -3714,9 +4217,15 @@
       <c r="G63" s="1">
         <v>6</v>
       </c>
-      <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
-      <c r="J63" s="8"/>
+      <c r="H63" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I63" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="J63" s="8" t="s">
+        <v>158</v>
+      </c>
       <c r="K63" s="9"/>
       <c r="L63" s="10"/>
       <c r="M63" s="9" t="s">
@@ -3745,9 +4254,15 @@
       <c r="G64" s="1">
         <v>7</v>
       </c>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="8"/>
+      <c r="H64" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I64" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="J64" s="8" t="s">
+        <v>158</v>
+      </c>
       <c r="K64" s="9"/>
       <c r="L64" s="10"/>
       <c r="M64" s="9" t="s">
@@ -3776,9 +4291,15 @@
       <c r="G65" s="1">
         <v>8</v>
       </c>
-      <c r="H65" s="8"/>
-      <c r="I65" s="8"/>
-      <c r="J65" s="8"/>
+      <c r="H65" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I65" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="J65" s="8" t="s">
+        <v>158</v>
+      </c>
       <c r="K65" s="9"/>
       <c r="L65" s="10"/>
       <c r="M65" s="9" t="s">
@@ -3807,9 +4328,15 @@
       <c r="G66" s="1">
         <v>1</v>
       </c>
-      <c r="H66" s="8"/>
-      <c r="I66" s="9"/>
-      <c r="J66" s="8"/>
+      <c r="H66" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I66" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="J66" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="K66" s="9"/>
       <c r="L66" s="10"/>
       <c r="M66" s="9" t="s">
@@ -3838,9 +4365,15 @@
       <c r="G67" s="1">
         <v>2</v>
       </c>
-      <c r="H67" s="8"/>
-      <c r="I67" s="9"/>
-      <c r="J67" s="8"/>
+      <c r="H67" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I67" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="J67" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="K67" s="9"/>
       <c r="L67" s="10"/>
       <c r="M67" s="9" t="s">
@@ -3869,9 +4402,15 @@
       <c r="G68" s="1">
         <v>3</v>
       </c>
-      <c r="H68" s="8"/>
-      <c r="I68" s="9"/>
-      <c r="J68" s="8"/>
+      <c r="H68" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I68" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="J68" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="K68" s="9"/>
       <c r="L68" s="10"/>
       <c r="M68" s="9" t="s">
@@ -3900,9 +4439,15 @@
       <c r="G69" s="1">
         <v>4</v>
       </c>
-      <c r="H69" s="8"/>
-      <c r="I69" s="9"/>
-      <c r="J69" s="8"/>
+      <c r="H69" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I69" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="J69" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="K69" s="9"/>
       <c r="L69" s="10"/>
       <c r="M69" s="9" t="s">
@@ -3931,9 +4476,15 @@
       <c r="G70" s="1">
         <v>5</v>
       </c>
-      <c r="H70" s="8"/>
-      <c r="I70" s="9"/>
-      <c r="J70" s="8"/>
+      <c r="H70" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I70" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="J70" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="K70" s="9"/>
       <c r="L70" s="10"/>
       <c r="M70" s="9" t="s">
@@ -3962,9 +4513,15 @@
       <c r="G71" s="1">
         <v>6</v>
       </c>
-      <c r="H71" s="8"/>
-      <c r="I71" s="9"/>
-      <c r="J71" s="8"/>
+      <c r="H71" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I71" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="J71" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="K71" s="9"/>
       <c r="L71" s="10"/>
       <c r="M71" s="9" t="s">
@@ -3993,9 +4550,15 @@
       <c r="G72" s="1">
         <v>7</v>
       </c>
-      <c r="H72" s="8"/>
-      <c r="I72" s="9"/>
-      <c r="J72" s="8"/>
+      <c r="H72" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I72" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="J72" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="K72" s="9"/>
       <c r="L72" s="10"/>
       <c r="M72" s="9" t="s">
@@ -4024,9 +4587,15 @@
       <c r="G73" s="1">
         <v>8</v>
       </c>
-      <c r="H73" s="8"/>
-      <c r="I73" s="9"/>
-      <c r="J73" s="8"/>
+      <c r="H73" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I73" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="J73" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="K73" s="9"/>
       <c r="L73" s="10"/>
       <c r="M73" s="9" t="s">
@@ -4055,10 +4624,15 @@
       <c r="G74" s="1">
         <v>1</v>
       </c>
-      <c r="H74" s="11"/>
-      <c r="I74" s="8"/>
-      <c r="J74" s="8"/>
-      <c r="K74" s="9"/>
+      <c r="H74" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I74" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J74" t="s">
+        <v>159</v>
+      </c>
       <c r="L74" s="10"/>
       <c r="M74" s="9" t="s">
         <v>89</v>
@@ -4086,10 +4660,15 @@
       <c r="G75" s="1">
         <v>2</v>
       </c>
-      <c r="H75" s="11"/>
-      <c r="I75" s="8"/>
-      <c r="J75" s="8"/>
-      <c r="K75" s="9"/>
+      <c r="H75" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I75" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J75" t="s">
+        <v>159</v>
+      </c>
       <c r="L75" s="10"/>
       <c r="M75" s="9" t="s">
         <v>90</v>
@@ -4117,10 +4696,16 @@
       <c r="G76" s="1">
         <v>3</v>
       </c>
-      <c r="H76" s="11"/>
-      <c r="I76" s="8"/>
-      <c r="J76" s="8"/>
-      <c r="K76" s="9"/>
+      <c r="H76" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I76" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J76" t="s">
+        <v>159</v>
+      </c>
+      <c r="K76" s="25"/>
       <c r="L76" s="10"/>
       <c r="M76" s="9" t="s">
         <v>91</v>
@@ -4148,9 +4733,15 @@
       <c r="G77" s="1">
         <v>4</v>
       </c>
-      <c r="H77" s="11"/>
-      <c r="I77" s="8"/>
-      <c r="J77" s="8"/>
+      <c r="H77" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I77" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J77" t="s">
+        <v>159</v>
+      </c>
       <c r="K77" s="9"/>
       <c r="L77" s="10"/>
       <c r="M77" s="9" t="s">
@@ -4179,9 +4770,15 @@
       <c r="G78" s="1">
         <v>5</v>
       </c>
-      <c r="H78" s="11"/>
-      <c r="I78" s="8"/>
-      <c r="J78" s="8"/>
+      <c r="H78" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I78" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J78" t="s">
+        <v>159</v>
+      </c>
       <c r="K78" s="9"/>
       <c r="L78" s="10"/>
       <c r="M78" s="9" t="s">
@@ -4210,9 +4807,15 @@
       <c r="G79" s="1">
         <v>6</v>
       </c>
-      <c r="H79" s="11"/>
-      <c r="I79" s="8"/>
-      <c r="J79" s="8"/>
+      <c r="H79" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I79" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J79" t="s">
+        <v>159</v>
+      </c>
       <c r="K79" s="9"/>
       <c r="L79" s="10"/>
       <c r="M79" s="9" t="s">
@@ -4241,9 +4844,15 @@
       <c r="G80" s="1">
         <v>7</v>
       </c>
-      <c r="H80" s="11"/>
-      <c r="I80" s="8"/>
-      <c r="J80" s="8"/>
+      <c r="H80" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I80" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J80" t="s">
+        <v>159</v>
+      </c>
       <c r="K80" s="9"/>
       <c r="L80" s="10"/>
       <c r="M80" s="9" t="s">
@@ -4272,9 +4881,15 @@
       <c r="G81" s="1">
         <v>8</v>
       </c>
-      <c r="H81" s="11"/>
-      <c r="I81" s="8"/>
-      <c r="J81" s="8"/>
+      <c r="H81" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I81" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J81" t="s">
+        <v>159</v>
+      </c>
       <c r="K81" s="9"/>
       <c r="L81" s="10"/>
       <c r="M81" s="9" t="s">
@@ -4301,9 +4916,15 @@
       <c r="G82" s="1">
         <v>1</v>
       </c>
-      <c r="H82" s="8"/>
-      <c r="I82" s="8"/>
-      <c r="J82" s="8"/>
+      <c r="H82" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I82" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="J82" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="K82" s="9"/>
       <c r="L82" s="10"/>
       <c r="M82" s="9" t="s">
@@ -4332,9 +4953,15 @@
       <c r="G83" s="1">
         <v>2</v>
       </c>
-      <c r="H83" s="8"/>
-      <c r="I83" s="8"/>
-      <c r="J83" s="8"/>
+      <c r="H83" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I83" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="J83" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="K83" s="9"/>
       <c r="L83" s="10"/>
       <c r="M83" s="9" t="s">
@@ -4363,9 +4990,15 @@
       <c r="G84" s="1">
         <v>3</v>
       </c>
-      <c r="H84" s="8"/>
-      <c r="I84" s="8"/>
-      <c r="J84" s="8"/>
+      <c r="H84" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I84" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="J84" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="K84" s="9"/>
       <c r="L84" s="10"/>
       <c r="M84" s="9" t="s">
@@ -4394,9 +5027,15 @@
       <c r="G85" s="1">
         <v>4</v>
       </c>
-      <c r="H85" s="8"/>
-      <c r="I85" s="8"/>
-      <c r="J85" s="8"/>
+      <c r="H85" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I85" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="J85" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="K85" s="9"/>
       <c r="L85" s="10"/>
       <c r="M85" s="9" t="s">
@@ -4425,9 +5064,15 @@
       <c r="G86" s="1">
         <v>5</v>
       </c>
-      <c r="H86" s="8"/>
-      <c r="I86" s="8"/>
-      <c r="J86" s="8"/>
+      <c r="H86" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I86" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="J86" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="K86" s="9"/>
       <c r="L86" s="10"/>
       <c r="M86" s="9" t="s">
@@ -4456,9 +5101,15 @@
       <c r="G87" s="1">
         <v>6</v>
       </c>
-      <c r="H87" s="8"/>
-      <c r="I87" s="8"/>
-      <c r="J87" s="8"/>
+      <c r="H87" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I87" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="J87" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="K87" s="9"/>
       <c r="L87" s="10"/>
       <c r="M87" s="9" t="s">
@@ -4487,9 +5138,15 @@
       <c r="G88" s="1">
         <v>7</v>
       </c>
-      <c r="H88" s="8"/>
-      <c r="I88" s="8"/>
-      <c r="J88" s="8"/>
+      <c r="H88" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I88" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="J88" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="K88" s="9"/>
       <c r="L88" s="10"/>
       <c r="M88" s="9" t="s">
@@ -4518,9 +5175,15 @@
       <c r="G89" s="1">
         <v>8</v>
       </c>
-      <c r="H89" s="8"/>
-      <c r="I89" s="8"/>
-      <c r="J89" s="8"/>
+      <c r="H89" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I89" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="J89" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="K89" s="9"/>
       <c r="L89" s="10"/>
       <c r="M89" s="9" t="s">
@@ -4549,9 +5212,15 @@
       <c r="G90" s="1">
         <v>1</v>
       </c>
-      <c r="H90" s="11"/>
-      <c r="I90" s="8"/>
-      <c r="J90" s="8"/>
+      <c r="H90" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I90" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="J90" s="8" t="s">
+        <v>160</v>
+      </c>
       <c r="K90" s="9"/>
       <c r="L90" s="10"/>
       <c r="M90" s="9" t="s">
@@ -4580,9 +5249,15 @@
       <c r="G91" s="1">
         <v>2</v>
       </c>
-      <c r="H91" s="11"/>
-      <c r="I91" s="8"/>
-      <c r="J91" s="8"/>
+      <c r="H91" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I91" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="J91" s="8" t="s">
+        <v>160</v>
+      </c>
       <c r="K91" s="9"/>
       <c r="L91" s="10"/>
       <c r="M91" s="9" t="s">
@@ -4611,9 +5286,15 @@
       <c r="G92" s="1">
         <v>3</v>
       </c>
-      <c r="H92" s="11"/>
-      <c r="I92" s="8"/>
-      <c r="J92" s="8"/>
+      <c r="H92" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I92" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="J92" s="8" t="s">
+        <v>160</v>
+      </c>
       <c r="K92" s="9"/>
       <c r="L92" s="10"/>
       <c r="M92" s="9" t="s">
@@ -4642,9 +5323,15 @@
       <c r="G93" s="1">
         <v>5</v>
       </c>
-      <c r="H93" s="11"/>
-      <c r="I93" s="8"/>
-      <c r="J93" s="8"/>
+      <c r="H93" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I93" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="J93" s="8" t="s">
+        <v>160</v>
+      </c>
       <c r="K93" s="9"/>
       <c r="L93" s="10"/>
       <c r="M93" s="9" t="s">
@@ -4673,9 +5360,15 @@
       <c r="G94" s="1">
         <v>6</v>
       </c>
-      <c r="H94" s="11"/>
-      <c r="I94" s="8"/>
-      <c r="J94" s="8"/>
+      <c r="H94" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I94" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="J94" s="8" t="s">
+        <v>160</v>
+      </c>
       <c r="K94" s="9"/>
       <c r="L94" s="10"/>
       <c r="M94" s="9" t="s">
@@ -4704,9 +5397,15 @@
       <c r="G95" s="1">
         <v>7</v>
       </c>
-      <c r="H95" s="11"/>
-      <c r="I95" s="8"/>
-      <c r="J95" s="8"/>
+      <c r="H95" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I95" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="J95" s="8" t="s">
+        <v>160</v>
+      </c>
       <c r="K95" s="9"/>
       <c r="L95" s="10"/>
       <c r="M95" s="9" t="s">

</xml_diff>

<commit_message>
cleanup full exp 1-2
</commit_message>
<xml_diff>
--- a/data/exp1.2/2023_Aug18_salbutamolexp1_2_meta.xlsx
+++ b/data/exp1.2/2023_Aug18_salbutamolexp1_2_meta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karissabarthelson/Documents/2023_MPSIII_salbutamol/data/exp1.2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983D05AB-4166-4B4B-A3E3-7A1E07F452DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9612DE9-B5E7-7645-916D-FD50ABEA735D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38560" yWindow="-11760" windowWidth="25000" windowHeight="19320" xr2:uid="{BD720F60-64AD-4D4B-861E-3C9FD6A3C16A}"/>
+    <workbookView xWindow="51800" yWindow="460" windowWidth="25000" windowHeight="15540" xr2:uid="{BD720F60-64AD-4D4B-861E-3C9FD6A3C16A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1878,9 +1878,9 @@
   </sheetPr>
   <dimension ref="A1:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J91" sqref="J91:J95"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>